<commit_message>
begain data analysis for pintle test
</commit_message>
<xml_diff>
--- a/analysis/Pressure Calibration/Calibration Plot.xlsx
+++ b/analysis/Pressure Calibration/Calibration Plot.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam-n-Abbs\Documents\GitHub\liquid-engine-test-stand\analysis\Pressure Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jntil\Documents\Git_Repos\liquid-engine-test-stand\analysis\Pressure Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED6F36F-2CEA-4109-BE20-263FBE6F8FF6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7587489-B386-42D0-8D07-F416DB97D91C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9465" xr2:uid="{B7A753EB-5698-4283-A025-AF9E9271D64A}"/>
   </bookViews>
@@ -55,13 +55,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,8 +89,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,23 +689,26 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
@@ -705,23 +716,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$7</c:f>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>818.01628664495104</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1060</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1149</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1303</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1462</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1553</c:v>
                 </c:pt>
               </c:numCache>
@@ -822,7 +836,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
+              <c:f>Sheet1!$A$4:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -846,7 +860,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$7</c:f>
+              <c:f>Sheet1!$C$4:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -963,7 +977,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
+              <c:f>Sheet1!$A$4:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -987,7 +1001,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$7</c:f>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1104,7 +1118,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
+              <c:f>Sheet1!$A$4:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1128,7 +1142,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$7</c:f>
+              <c:f>Sheet1!$E$4:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1245,7 +1259,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
+              <c:f>Sheet1!$A$4:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1269,7 +1283,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$7</c:f>
+              <c:f>Sheet1!$F$4:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3200,13 +3214,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3236,13 +3250,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3278,7 +3292,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3604,10 +3618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861754D1-121F-4A0C-BB06-B4BFE0437546}">
-  <dimension ref="A2:F7"/>
+  <dimension ref="A2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3638,101 +3652,109 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>37</v>
+        <v>0</v>
       </c>
-      <c r="B3">
-        <v>1060</v>
-      </c>
-      <c r="C3">
-        <v>293.8</v>
-      </c>
-      <c r="D3">
-        <v>719</v>
-      </c>
-      <c r="E3">
-        <v>254.3</v>
-      </c>
-      <c r="F3">
-        <v>833.8</v>
+      <c r="B3" s="1">
+        <v>818.01628664495104</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B4">
-        <v>1149</v>
+        <v>1060</v>
       </c>
       <c r="C4">
-        <v>319.5</v>
+        <v>293.8</v>
       </c>
       <c r="D4">
-        <v>782.3</v>
+        <v>719</v>
       </c>
       <c r="E4">
-        <v>275.2</v>
+        <v>254.3</v>
       </c>
       <c r="F4">
-        <v>847.4</v>
+        <v>833.8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="B5">
-        <v>1303</v>
+        <v>1149</v>
       </c>
       <c r="C5">
-        <v>366.2</v>
+        <v>319.5</v>
       </c>
       <c r="D5">
-        <v>887.2</v>
+        <v>782.3</v>
       </c>
       <c r="E5">
-        <v>309.5</v>
+        <v>275.2</v>
       </c>
       <c r="F5">
-        <v>876.1</v>
+        <v>847.4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B6">
-        <v>1462</v>
+        <v>1303</v>
       </c>
       <c r="C6">
-        <v>406.3</v>
+        <v>366.2</v>
       </c>
       <c r="D6">
-        <v>973.9</v>
+        <v>887.2</v>
       </c>
       <c r="E6">
-        <v>337.1</v>
+        <v>309.5</v>
       </c>
       <c r="F6">
-        <v>895.9</v>
+        <v>876.1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <v>1462</v>
+      </c>
+      <c r="C7">
+        <v>406.3</v>
+      </c>
+      <c r="D7">
+        <v>973.9</v>
+      </c>
+      <c r="E7">
+        <v>337.1</v>
+      </c>
+      <c r="F7">
+        <v>895.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>120</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>1553</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>443.7</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>1057</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>371.5</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>918.1</v>
       </c>
     </row>

</xml_diff>